<commit_message>
Update all assignment 1 files
</commit_message>
<xml_diff>
--- a/Assignment 1/G1_Acceptance.Ass1.xlsx
+++ b/Assignment 1/G1_Acceptance.Ass1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/benaya_leib_e_braude_ac_il/Documents/Braude/קורסים/שנה ד'/שיטות הנדסיות לפיתוח מערכות תוכנה/מטלות הגשה/מטלה 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\backed up stuff\temp studies\שיטות\G1_Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="584" documentId="13_ncr:1_{11DF0857-C96A-47CC-B99D-03A1C275CFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B90A0A2-14FE-4E39-B80A-570DD63DABDA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7018E13-7789-469C-ADF4-69718424DFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="300" windowWidth="21600" windowHeight="11295" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="161">
   <si>
     <t>נתן נימיץ</t>
   </si>
@@ -538,17 +538,23 @@
   </si>
   <si>
     <t>System shows the requested report.</t>
+  </si>
+  <si>
+    <t>תומר חנניה</t>
+  </si>
+  <si>
+    <t>Tomer.Hananya@e.braude.ac.il</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -562,7 +568,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -570,7 +576,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -644,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,10 +676,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -688,18 +694,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -998,498 +998,506 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="23">
         <v>45819</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="20">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
         <v>1</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5">
-      <c r="A7" s="20">
+    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
         <v>2</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="20">
+      <c r="C8" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
         <v>3</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="20">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.5">
-      <c r="A10" s="20">
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.5">
-      <c r="A11" s="20">
+      <c r="C11" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
         <v>4.2</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="20">
+      <c r="C12" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
         <v>5</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.5">
-      <c r="A13" s="20">
+    <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="20">
+      <c r="C14" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
         <v>5.2</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.5">
-      <c r="A15" s="20">
+      <c r="C15" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
         <v>5.3</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="20">
+      <c r="C16" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
         <v>6</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C17" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="20">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
         <v>6.1</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="20">
+      <c r="C18" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
         <v>6.2</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="20">
+      <c r="C19" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
         <v>6.3</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="20">
+      <c r="C20" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
         <v>6.4</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="20">
+      <c r="C21" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
         <v>7</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C22" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="20">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
         <v>7.1</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="20">
+      <c r="C23" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
         <v>8</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B24" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="20">
+    <row r="25" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
         <v>8.1</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="20">
+      <c r="C25" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="20">
+      <c r="C26" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
         <v>9</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B27" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C27" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="20">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
         <v>10</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C28" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="20">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
         <v>10.1</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="20">
+      <c r="C29" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
         <v>10.199999999999999</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B30" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="20">
+      <c r="C30" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
         <v>11</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B31" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C31" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="20">
+    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
         <v>11.1</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B32" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="20">
+      <c r="C32" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
         <v>12</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B33" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C33" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="20">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
         <v>13</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B34" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C34" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="28.5">
-      <c r="A34" s="20">
+    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
         <v>13.1</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B35" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="20">
+      <c r="C35" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="18">
         <v>14</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B36" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C36" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="20">
-        <v>15</v>
-      </c>
-      <c r="B36" s="22" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <v>15</v>
+      </c>
+      <c r="B37" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C37" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="20">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
         <v>16</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B38" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C38" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="20">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
         <v>16.100000000000001</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B39" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="20">
+      <c r="C39" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="18">
         <v>16.2</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="20">
+      <c r="C40" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
         <v>16.3</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B41" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="20">
+      <c r="C41" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="18">
         <v>17</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B42" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C42" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="29.1" customHeight="1">
-      <c r="A42" s="20">
+    <row r="43" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
         <v>17.100000000000001</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B43" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="28.5">
-      <c r="A43" s="20" t="s">
+      <c r="C43" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B44" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="28.5">
-      <c r="A44" s="20" t="s">
+      <c r="C44" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B45" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C45" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1514,16 +1522,16 @@
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5" customWidth="1"/>
-    <col min="2" max="2" width="37.75" customWidth="1"/>
-    <col min="3" max="3" width="43.125" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.875" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>55</v>
       </c>
@@ -1540,7 +1548,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>60</v>
       </c>
@@ -1557,7 +1565,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>65</v>
       </c>
@@ -1574,7 +1582,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="56.25">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>67</v>
       </c>
@@ -1591,7 +1599,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="70.5">
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>72</v>
       </c>
@@ -1608,7 +1616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="98.25">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>76</v>
       </c>
@@ -1625,7 +1633,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>80</v>
       </c>
@@ -1642,7 +1650,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="42">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>85</v>
       </c>
@@ -1659,7 +1667,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="42">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>88</v>
       </c>
@@ -1676,7 +1684,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>93</v>
       </c>
@@ -1693,7 +1701,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.5">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>97</v>
       </c>
@@ -1710,7 +1718,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.5">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>101</v>
       </c>
@@ -1727,7 +1735,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="42">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>104</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.5">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>107</v>
       </c>
@@ -1761,7 +1769,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="42">
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>112</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="42">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>117</v>
       </c>
@@ -1795,7 +1803,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>121</v>
       </c>
@@ -1812,7 +1820,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.5">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>126</v>
       </c>
@@ -1829,7 +1837,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>130</v>
       </c>
@@ -1846,7 +1854,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28.5">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>135</v>
       </c>
@@ -1863,7 +1871,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.5">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>139</v>
       </c>
@@ -1880,7 +1888,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1899,16 +1907,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5" customWidth="1"/>
-    <col min="2" max="2" width="39.5" customWidth="1"/>
-    <col min="3" max="3" width="39.75" customWidth="1"/>
-    <col min="4" max="4" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>55</v>
       </c>
@@ -1925,7 +1933,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>60</v>
       </c>
@@ -1942,7 +1950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>65</v>
       </c>
@@ -1959,7 +1967,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30.75">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>144</v>
       </c>
@@ -1976,299 +1984,299 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.5">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" ht="15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" ht="15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" ht="15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" ht="15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" ht="15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" ht="15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" ht="15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:5" ht="15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" ht="15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="1:5" ht="15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" ht="15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" ht="15">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>

</xml_diff>